<commit_message>
Testing function for Circuit class, also edited excel file as there was error in one case.
</commit_message>
<xml_diff>
--- a/InputOutputTable.xlsx
+++ b/InputOutputTable.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS Study\CMPE 202 Software Systems Engineering[Prof. Paul Nguyen]\Team Project(Kanban)[CryptoUnpluggers]\CryptoUnpluggers\CMPE202-CSUnplugged-PeruvianFlipCoin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -86,13 +86,13 @@
     <t>1 0 0 0 0 1</t>
   </si>
   <si>
-    <t>1 1 1 1 0 0</t>
+    <t xml:space="preserve">0 1 0 1 0 1 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,18 +184,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -505,15 +494,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G9"/>
+  <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -541,7 +530,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -561,7 +550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -569,27 +558,28 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -597,7 +587,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Tester function for Circuit Three, changes in circuit class and changes in Excel sheet for wrong outputs
</commit_message>
<xml_diff>
--- a/InputOutputTable.xlsx
+++ b/InputOutputTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Input</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>1 1 1 0 0 0</t>
-  </si>
-  <si>
-    <t>1 0 0 1 0 1</t>
   </si>
   <si>
     <t>0 0 0 1 0 1</t>
@@ -497,7 +494,7 @@
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,19 +557,19 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -595,13 +592,13 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Tester function for Circuit Four and changed the Excel sheet for wrong outputs given and necessary changes in circuit class.
</commit_message>
<xml_diff>
--- a/InputOutputTable.xlsx
+++ b/InputOutputTable.xlsx
@@ -494,7 +494,7 @@
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Testing function for Fifth Circuit with changes in Excel sheet for wrong inputs given
</commit_message>
<xml_diff>
--- a/InputOutputTable.xlsx
+++ b/InputOutputTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Input</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">0 1 0 1 0 1 </t>
+  </si>
+  <si>
+    <t>1 1 1 1 0 0</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1"/>
     </row>

</xml_diff>